<commit_message>
Sta sad ne valja :D
</commit_message>
<xml_diff>
--- a/imena.xlsx
+++ b/imena.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Names" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -28,12 +28,6 @@
     <t>Rodnic</t>
   </si>
   <si>
-    <t>Vala</t>
-  </si>
-  <si>
-    <t>Valic</t>
-  </si>
-  <si>
     <t>Roki</t>
   </si>
   <si>
@@ -44,6 +38,12 @@
   </si>
   <si>
     <t>Krakic</t>
+  </si>
+  <si>
+    <t>Rada</t>
+  </si>
+  <si>
+    <t>Radic</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,26 +411,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mislim da sam namestio sad po svakom pokretanju procita sva imena i doda jos pet i onda iscita sva imena sa njima takodje
</commit_message>
<xml_diff>
--- a/imena.xlsx
+++ b/imena.xlsx
@@ -34,16 +34,16 @@
     <t>Rokic</t>
   </si>
   <si>
-    <t>Krako</t>
-  </si>
-  <si>
-    <t>Krakic</t>
-  </si>
-  <si>
     <t>Rada</t>
   </si>
   <si>
     <t>Radic</t>
+  </si>
+  <si>
+    <t>Wynell</t>
+  </si>
+  <si>
+    <t>Aufderhar</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B16" sqref="A6:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,10 +411,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -427,10 +427,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stari ispisi plus pet novih posevno ispisani sa razmakom
</commit_message>
<xml_diff>
--- a/imena.xlsx
+++ b/imena.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Milan</t>
   </si>
@@ -44,12 +44,163 @@
   </si>
   <si>
     <t>Aufderhar</t>
+  </si>
+  <si>
+    <t>Reuben</t>
+  </si>
+  <si>
+    <t>Homenick</t>
+  </si>
+  <si>
+    <t>Merri</t>
+  </si>
+  <si>
+    <t>Reichel</t>
+  </si>
+  <si>
+    <t>Collette</t>
+  </si>
+  <si>
+    <t>Lynch</t>
+  </si>
+  <si>
+    <t>Jonna</t>
+  </si>
+  <si>
+    <t>Beier</t>
+  </si>
+  <si>
+    <t>Wilburn</t>
+  </si>
+  <si>
+    <t>Franecki</t>
+  </si>
+  <si>
+    <t>Cyrstal</t>
+  </si>
+  <si>
+    <t>Kovacek</t>
+  </si>
+  <si>
+    <t>Robt</t>
+  </si>
+  <si>
+    <t>Hermiston</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>McKenzie</t>
+  </si>
+  <si>
+    <t>Narcisa</t>
+  </si>
+  <si>
+    <t>Lebsack</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Fritsch</t>
+  </si>
+  <si>
+    <t>Michal</t>
+  </si>
+  <si>
+    <t>Greenholt</t>
+  </si>
+  <si>
+    <t>Kareem</t>
+  </si>
+  <si>
+    <t>Hauck</t>
+  </si>
+  <si>
+    <t>Barrett</t>
+  </si>
+  <si>
+    <t>Wyman</t>
+  </si>
+  <si>
+    <t>Robby</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Clarine</t>
+  </si>
+  <si>
+    <t>Luettgen</t>
+  </si>
+  <si>
+    <t>Emmaline</t>
+  </si>
+  <si>
+    <t>Hammes</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Hegmann</t>
+  </si>
+  <si>
+    <t>Ward</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>Sanford</t>
+  </si>
+  <si>
+    <t>Lakin</t>
+  </si>
+  <si>
+    <t>Flavia</t>
+  </si>
+  <si>
+    <t>Upton</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>Rickie</t>
+  </si>
+  <si>
+    <t>Brekke</t>
+  </si>
+  <si>
+    <t>Amado</t>
+  </si>
+  <si>
+    <t>Powlowski</t>
+  </si>
+  <si>
+    <t>Royal</t>
+  </si>
+  <si>
+    <t>Windler</t>
+  </si>
+  <si>
+    <t>Peg</t>
+  </si>
+  <si>
+    <t>Yost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="A6:B16"/>
@@ -394,43 +545,243 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>